<commit_message>
Update B4P Engine Guide
</commit_message>
<xml_diff>
--- a/Images/Stock Market Listing.xlsx
+++ b/Images/Stock Market Listing.xlsx
@@ -6365,13 +6365,13 @@
         <v>227</v>
       </c>
       <c r="D111" s="4">
-        <v>61.43</v>
+        <v>60.69</v>
       </c>
       <c r="E111" s="5">
-        <v>0</v>
+        <v>-0.74</v>
       </c>
       <c r="F111" s="6">
-        <v>0</v>
+        <v>-0.012</v>
       </c>
       <c r="G111" s="4">
         <v>0.022182</v>
@@ -6437,13 +6437,13 @@
         <v>233</v>
       </c>
       <c r="D114" s="4">
-        <v>81.69</v>
-      </c>
-      <c r="E114" s="5">
-        <v>0</v>
-      </c>
-      <c r="F114" s="6">
-        <v>0</v>
+        <v>82.15</v>
+      </c>
+      <c r="E114" s="12">
+        <v>0.46</v>
+      </c>
+      <c r="F114" s="13">
+        <v>0.0056</v>
       </c>
       <c r="G114" s="4">
         <v>0.315752</v>
@@ -6975,13 +6975,13 @@
         <v>277</v>
       </c>
       <c r="D136" s="7">
-        <v>244.46</v>
+        <v>244.45</v>
       </c>
       <c r="E136" s="8">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="F136" s="9">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="G136" s="7">
         <v>0.104511</v>
@@ -7099,13 +7099,13 @@
         <v>287</v>
       </c>
       <c r="D141" s="7">
-        <v>59.64</v>
-      </c>
-      <c r="E141" s="8">
-        <v>0</v>
-      </c>
-      <c r="F141" s="9">
-        <v>0</v>
+        <v>60</v>
+      </c>
+      <c r="E141" s="10">
+        <v>0.36</v>
+      </c>
+      <c r="F141" s="11">
+        <v>0.006</v>
       </c>
       <c r="G141" s="7">
         <v>0.112519</v>
@@ -7149,13 +7149,13 @@
         <v>291</v>
       </c>
       <c r="D143" s="4">
-        <v>28.75</v>
-      </c>
-      <c r="E143" s="5">
-        <v>0</v>
-      </c>
-      <c r="F143" s="6">
-        <v>0</v>
+        <v>28.76</v>
+      </c>
+      <c r="E143" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="F143" s="13">
+        <v>0.0003</v>
       </c>
       <c r="G143" s="4">
         <v>0.056998</v>
@@ -8067,13 +8067,13 @@
         <v>367</v>
       </c>
       <c r="D181" s="7">
-        <v>311.69</v>
-      </c>
-      <c r="E181" s="8">
-        <v>0</v>
-      </c>
-      <c r="F181" s="9">
-        <v>0</v>
+        <v>311.89</v>
+      </c>
+      <c r="E181" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="F181" s="11">
+        <v>0.0006</v>
       </c>
       <c r="G181" s="7">
         <v>0.643899</v>
@@ -8501,13 +8501,13 @@
         <v>403</v>
       </c>
       <c r="D199" s="4">
-        <v>86.84</v>
-      </c>
-      <c r="E199" s="5">
-        <v>0</v>
-      </c>
-      <c r="F199" s="6">
-        <v>0</v>
+        <v>86.97</v>
+      </c>
+      <c r="E199" s="12">
+        <v>0.13</v>
+      </c>
+      <c r="F199" s="13">
+        <v>0.0015</v>
       </c>
       <c r="G199" s="4">
         <v>0.946754</v>
@@ -9059,13 +9059,13 @@
         <v>449</v>
       </c>
       <c r="D222" s="4">
-        <v>287.41</v>
-      </c>
-      <c r="E222" s="5">
-        <v>0</v>
-      </c>
-      <c r="F222" s="6">
-        <v>0</v>
+        <v>287.5</v>
+      </c>
+      <c r="E222" s="12">
+        <v>0.09</v>
+      </c>
+      <c r="F222" s="13">
+        <v>0.0003</v>
       </c>
       <c r="G222" s="4">
         <v>0.049093</v>
@@ -10611,13 +10611,13 @@
         <v>577</v>
       </c>
       <c r="D286" s="4">
-        <v>19.48</v>
-      </c>
-      <c r="E286" s="5">
-        <v>0</v>
-      </c>
-      <c r="F286" s="6">
-        <v>0</v>
+        <v>19.49</v>
+      </c>
+      <c r="E286" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="F286" s="13">
+        <v>0.0005</v>
       </c>
       <c r="G286" s="4">
         <v>0.098395</v>
@@ -10807,13 +10807,13 @@
         <v>593</v>
       </c>
       <c r="D294" s="4">
-        <v>35.95</v>
-      </c>
-      <c r="E294" s="5">
-        <v>0</v>
-      </c>
-      <c r="F294" s="6">
-        <v>0</v>
+        <v>35.99</v>
+      </c>
+      <c r="E294" s="12">
+        <v>0.04</v>
+      </c>
+      <c r="F294" s="13">
+        <v>0.0011</v>
       </c>
       <c r="G294" s="4">
         <v>0.032642</v>
@@ -10855,13 +10855,13 @@
         <v>597</v>
       </c>
       <c r="D296" s="7">
-        <v>74.92</v>
-      </c>
-      <c r="E296" s="8">
-        <v>0</v>
-      </c>
-      <c r="F296" s="9">
-        <v>0</v>
+        <v>75.44</v>
+      </c>
+      <c r="E296" s="10">
+        <v>0.52</v>
+      </c>
+      <c r="F296" s="11">
+        <v>0.0069</v>
       </c>
       <c r="G296" s="7">
         <v>0.051317</v>
@@ -10951,13 +10951,13 @@
         <v>605</v>
       </c>
       <c r="D300" s="7">
-        <v>461.52</v>
+        <v>461.25</v>
       </c>
       <c r="E300" s="8">
-        <v>0</v>
+        <v>-0.27</v>
       </c>
       <c r="F300" s="9">
-        <v>0</v>
+        <v>-0.0006</v>
       </c>
       <c r="G300" s="7">
         <v>0.296659</v>
@@ -11071,13 +11071,13 @@
         <v>615</v>
       </c>
       <c r="D305" s="7">
-        <v>11.36</v>
-      </c>
-      <c r="E305" s="8">
-        <v>0</v>
-      </c>
-      <c r="F305" s="9">
-        <v>0</v>
+        <v>11.39</v>
+      </c>
+      <c r="E305" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="F305" s="11">
+        <v>0.0026</v>
       </c>
       <c r="G305" s="7">
         <v>0.027559</v>
@@ -11095,13 +11095,13 @@
         <v>617</v>
       </c>
       <c r="D306" s="4">
-        <v>101.53</v>
-      </c>
-      <c r="E306" s="5">
-        <v>0</v>
-      </c>
-      <c r="F306" s="6">
-        <v>0</v>
+        <v>102</v>
+      </c>
+      <c r="E306" s="12">
+        <v>0.47</v>
+      </c>
+      <c r="F306" s="13">
+        <v>0.0046</v>
       </c>
       <c r="G306" s="4">
         <v>0.069265</v>
@@ -11143,13 +11143,13 @@
         <v>621</v>
       </c>
       <c r="D308" s="7">
-        <v>39.2</v>
-      </c>
-      <c r="E308" s="8">
-        <v>0</v>
-      </c>
-      <c r="F308" s="9">
-        <v>0</v>
+        <v>39.45</v>
+      </c>
+      <c r="E308" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="F308" s="11">
+        <v>0.0064</v>
       </c>
       <c r="G308" s="7">
         <v>0.038803</v>
@@ -11167,13 +11167,13 @@
         <v>623</v>
       </c>
       <c r="D309" s="7">
-        <v>506.49</v>
+        <v>503.8</v>
       </c>
       <c r="E309" s="8">
-        <v>0</v>
+        <v>-2.69</v>
       </c>
       <c r="F309" s="9">
-        <v>0</v>
+        <v>-0.0053</v>
       </c>
       <c r="G309" s="7">
         <v>0.108955</v>
@@ -11215,13 +11215,13 @@
         <v>627</v>
       </c>
       <c r="D311" s="4">
-        <v>86.9</v>
-      </c>
-      <c r="E311" s="5">
-        <v>0</v>
-      </c>
-      <c r="F311" s="6">
-        <v>0</v>
+        <v>87.01</v>
+      </c>
+      <c r="E311" s="12">
+        <v>0.11</v>
+      </c>
+      <c r="F311" s="13">
+        <v>0.0013</v>
       </c>
       <c r="G311" s="4">
         <v>0.1307</v>
@@ -11459,13 +11459,13 @@
         <v>647</v>
       </c>
       <c r="D321" s="7">
-        <v>251.46</v>
-      </c>
-      <c r="E321" s="8">
-        <v>0</v>
-      </c>
-      <c r="F321" s="9">
-        <v>0</v>
+        <v>251.98</v>
+      </c>
+      <c r="E321" s="10">
+        <v>0.52</v>
+      </c>
+      <c r="F321" s="11">
+        <v>0.0021</v>
       </c>
       <c r="G321" s="7">
         <v>0.499767</v>
@@ -11507,13 +11507,13 @@
         <v>651</v>
       </c>
       <c r="D323" s="4">
-        <v>112.47</v>
+        <v>112.2</v>
       </c>
       <c r="E323" s="5">
-        <v>0</v>
+        <v>-0.27</v>
       </c>
       <c r="F323" s="6">
-        <v>0</v>
+        <v>-0.0024</v>
       </c>
       <c r="G323" s="4">
         <v>0.396723</v>
@@ -11579,13 +11579,13 @@
         <v>657</v>
       </c>
       <c r="D326" s="4">
-        <v>70.61</v>
-      </c>
-      <c r="E326" s="5">
-        <v>0</v>
-      </c>
-      <c r="F326" s="6">
-        <v>0</v>
+        <v>70.67</v>
+      </c>
+      <c r="E326" s="12">
+        <v>0.06</v>
+      </c>
+      <c r="F326" s="13">
+        <v>0.0008</v>
       </c>
       <c r="G326" s="4">
         <v>0.128321</v>
@@ -11977,13 +11977,13 @@
         <v>689</v>
       </c>
       <c r="D342" s="4">
-        <v>73.86</v>
-      </c>
-      <c r="E342" s="5">
-        <v>0</v>
-      </c>
-      <c r="F342" s="6">
-        <v>0</v>
+        <v>74.31</v>
+      </c>
+      <c r="E342" s="12">
+        <v>0.45</v>
+      </c>
+      <c r="F342" s="13">
+        <v>0.0061</v>
       </c>
       <c r="G342" s="4">
         <v>0.069522</v>
@@ -12343,13 +12343,13 @@
         <v>719</v>
       </c>
       <c r="D357" s="7">
-        <v>86.09</v>
+        <v>86</v>
       </c>
       <c r="E357" s="8">
-        <v>0</v>
+        <v>-0.09</v>
       </c>
       <c r="F357" s="9">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
       <c r="G357" s="7">
         <v>0.449265</v>
@@ -12391,13 +12391,13 @@
         <v>723</v>
       </c>
       <c r="D359" s="4">
-        <v>27.75</v>
+        <v>27.2</v>
       </c>
       <c r="E359" s="5">
-        <v>0</v>
+        <v>-0.55</v>
       </c>
       <c r="F359" s="6">
-        <v>0</v>
+        <v>-0.0198</v>
       </c>
       <c r="G359" s="4">
         <v>0.026202</v>
@@ -12535,13 +12535,13 @@
         <v>735</v>
       </c>
       <c r="D365" s="7">
-        <v>19.94</v>
-      </c>
-      <c r="E365" s="8">
-        <v>0</v>
-      </c>
-      <c r="F365" s="9">
-        <v>0</v>
+        <v>19.99</v>
+      </c>
+      <c r="E365" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="F365" s="11">
+        <v>0.0025</v>
       </c>
       <c r="G365" s="7">
         <v>0.022285</v>
@@ -12559,13 +12559,13 @@
         <v>737</v>
       </c>
       <c r="D366" s="4">
-        <v>150.76</v>
-      </c>
-      <c r="E366" s="5">
-        <v>0</v>
-      </c>
-      <c r="F366" s="6">
-        <v>0</v>
+        <v>150.99</v>
+      </c>
+      <c r="E366" s="12">
+        <v>0.23</v>
+      </c>
+      <c r="F366" s="13">
+        <v>0.0015</v>
       </c>
       <c r="G366" s="4">
         <v>0.107929</v>
@@ -12829,13 +12829,13 @@
         <v>759</v>
       </c>
       <c r="D377" s="7">
-        <v>184.7</v>
-      </c>
-      <c r="E377" s="8">
-        <v>0</v>
-      </c>
-      <c r="F377" s="9">
-        <v>0</v>
+        <v>184.83</v>
+      </c>
+      <c r="E377" s="10">
+        <v>0.13</v>
+      </c>
+      <c r="F377" s="11">
+        <v>0.0007</v>
       </c>
       <c r="G377" s="7">
         <v>0.200279</v>
@@ -13219,13 +13219,13 @@
         <v>791</v>
       </c>
       <c r="D393" s="7">
-        <v>55.17</v>
+        <v>55.12</v>
       </c>
       <c r="E393" s="8">
-        <v>0</v>
+        <v>-0.05</v>
       </c>
       <c r="F393" s="9">
-        <v>0</v>
+        <v>-0.0009</v>
       </c>
       <c r="G393" s="7">
         <v>0.814079</v>
@@ -13315,13 +13315,13 @@
         <v>799</v>
       </c>
       <c r="D397" s="7">
-        <v>78.84</v>
+        <v>78.5</v>
       </c>
       <c r="E397" s="8">
-        <v>0</v>
+        <v>-0.34</v>
       </c>
       <c r="F397" s="9">
-        <v>0</v>
+        <v>-0.0043</v>
       </c>
       <c r="G397" s="7">
         <v>0.023453</v>
@@ -13339,13 +13339,13 @@
         <v>801</v>
       </c>
       <c r="D398" s="4">
-        <v>254.11</v>
+        <v>253.99</v>
       </c>
       <c r="E398" s="5">
-        <v>0</v>
+        <v>-0.12</v>
       </c>
       <c r="F398" s="6">
-        <v>0</v>
+        <v>-0.0005</v>
       </c>
       <c r="G398" s="4">
         <v>0.145225</v>
@@ -13555,13 +13555,13 @@
         <v>819</v>
       </c>
       <c r="D407" s="4">
-        <v>40.67</v>
-      </c>
-      <c r="E407" s="5">
-        <v>0</v>
-      </c>
-      <c r="F407" s="6">
-        <v>0</v>
+        <v>41.19</v>
+      </c>
+      <c r="E407" s="12">
+        <v>0.52</v>
+      </c>
+      <c r="F407" s="13">
+        <v>0.0128</v>
       </c>
       <c r="G407" s="4">
         <v>0.02674</v>
@@ -13725,13 +13725,13 @@
         <v>833</v>
       </c>
       <c r="D414" s="4">
-        <v>100.4</v>
-      </c>
-      <c r="E414" s="5">
-        <v>0</v>
-      </c>
-      <c r="F414" s="6">
-        <v>0</v>
+        <v>100.49</v>
+      </c>
+      <c r="E414" s="12">
+        <v>0.09</v>
+      </c>
+      <c r="F414" s="13">
+        <v>0.0009</v>
       </c>
       <c r="G414" s="4">
         <v>0.396574</v>
@@ -14257,13 +14257,13 @@
         <v>877</v>
       </c>
       <c r="D436" s="7">
-        <v>169.79</v>
+        <v>169.75</v>
       </c>
       <c r="E436" s="8">
-        <v>0</v>
+        <v>-0.04</v>
       </c>
       <c r="F436" s="9">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="G436" s="7">
         <v>0.141106</v>
@@ -14281,13 +14281,13 @@
         <v>879</v>
       </c>
       <c r="D437" s="7">
-        <v>515.6</v>
+        <v>515</v>
       </c>
       <c r="E437" s="8">
-        <v>0</v>
+        <v>-0.6</v>
       </c>
       <c r="F437" s="9">
-        <v>0</v>
+        <v>-0.0012</v>
       </c>
       <c r="G437" s="7">
         <v>0.278602</v>
@@ -14475,13 +14475,13 @@
         <v>895</v>
       </c>
       <c r="D445" s="7">
-        <v>76.49</v>
-      </c>
-      <c r="E445" s="8">
-        <v>0</v>
-      </c>
-      <c r="F445" s="9">
-        <v>0</v>
+        <v>76.73</v>
+      </c>
+      <c r="E445" s="10">
+        <v>0.24</v>
+      </c>
+      <c r="F445" s="11">
+        <v>0.0031</v>
       </c>
       <c r="G445" s="7">
         <v>0.211119</v>
@@ -14499,13 +14499,13 @@
         <v>897</v>
       </c>
       <c r="D446" s="4">
-        <v>41.24</v>
+        <v>41.08</v>
       </c>
       <c r="E446" s="5">
-        <v>0</v>
+        <v>-0.16</v>
       </c>
       <c r="F446" s="6">
-        <v>0</v>
+        <v>-0.0039</v>
       </c>
       <c r="G446" s="4">
         <v>0.065699</v>
@@ -14621,13 +14621,13 @@
         <v>907</v>
       </c>
       <c r="D451" s="4">
-        <v>269.47</v>
-      </c>
-      <c r="E451" s="5">
-        <v>0</v>
-      </c>
-      <c r="F451" s="6">
-        <v>0</v>
+        <v>270</v>
+      </c>
+      <c r="E451" s="12">
+        <v>0.53</v>
+      </c>
+      <c r="F451" s="13">
+        <v>0.002</v>
       </c>
       <c r="G451" s="4">
         <v>0.238505</v>
@@ -14645,13 +14645,13 @@
         <v>909</v>
       </c>
       <c r="D452" s="7">
-        <v>36.64</v>
-      </c>
-      <c r="E452" s="8">
-        <v>0</v>
-      </c>
-      <c r="F452" s="9">
-        <v>0</v>
+        <v>36.95</v>
+      </c>
+      <c r="E452" s="10">
+        <v>0.31</v>
+      </c>
+      <c r="F452" s="11">
+        <v>0.0085</v>
       </c>
       <c r="G452" s="7">
         <v>0.048863</v>
@@ -14841,13 +14841,13 @@
         <v>925</v>
       </c>
       <c r="D460" s="7">
-        <v>33.25</v>
-      </c>
-      <c r="E460" s="8">
-        <v>0</v>
-      </c>
-      <c r="F460" s="9">
-        <v>0</v>
+        <v>33.49</v>
+      </c>
+      <c r="E460" s="10">
+        <v>0.24</v>
+      </c>
+      <c r="F460" s="11">
+        <v>0.0072</v>
       </c>
       <c r="G460" s="7">
         <v>0.023115</v>
@@ -14865,13 +14865,13 @@
         <v>927</v>
       </c>
       <c r="D461" s="7">
-        <v>233.34</v>
-      </c>
-      <c r="E461" s="8">
-        <v>0</v>
-      </c>
-      <c r="F461" s="9">
-        <v>0</v>
+        <v>233.5</v>
+      </c>
+      <c r="E461" s="10">
+        <v>0.16</v>
+      </c>
+      <c r="F461" s="11">
+        <v>0.0007</v>
       </c>
       <c r="G461" s="7">
         <v>0.287478</v>
@@ -15181,13 +15181,13 @@
         <v>953</v>
       </c>
       <c r="D474" s="4">
-        <v>53.87</v>
-      </c>
-      <c r="E474" s="5">
-        <v>0</v>
-      </c>
-      <c r="F474" s="6">
-        <v>0</v>
+        <v>54</v>
+      </c>
+      <c r="E474" s="12">
+        <v>0.13</v>
+      </c>
+      <c r="F474" s="13">
+        <v>0.0024</v>
       </c>
       <c r="G474" s="4">
         <v>0.188409</v>
@@ -15253,13 +15253,13 @@
         <v>959</v>
       </c>
       <c r="D477" s="7">
-        <v>92.44</v>
-      </c>
-      <c r="E477" s="8">
-        <v>0</v>
-      </c>
-      <c r="F477" s="9">
-        <v>0</v>
+        <v>92.5</v>
+      </c>
+      <c r="E477" s="10">
+        <v>0.06</v>
+      </c>
+      <c r="F477" s="11">
+        <v>0.0006</v>
       </c>
       <c r="G477" s="7">
         <v>0.070626</v>
@@ -15277,13 +15277,13 @@
         <v>961</v>
       </c>
       <c r="D478" s="4">
-        <v>52.25</v>
-      </c>
-      <c r="E478" s="5">
-        <v>0</v>
-      </c>
-      <c r="F478" s="6">
-        <v>0</v>
+        <v>52.54</v>
+      </c>
+      <c r="E478" s="12">
+        <v>0.29</v>
+      </c>
+      <c r="F478" s="13">
+        <v>0.0056</v>
       </c>
       <c r="G478" s="4">
         <v>0.186704</v>
@@ -15301,13 +15301,13 @@
         <v>963</v>
       </c>
       <c r="D479" s="4">
-        <v>58.74</v>
-      </c>
-      <c r="E479" s="5">
-        <v>0</v>
-      </c>
-      <c r="F479" s="6">
-        <v>0</v>
+        <v>58.81</v>
+      </c>
+      <c r="E479" s="12">
+        <v>0.07</v>
+      </c>
+      <c r="F479" s="13">
+        <v>0.0012</v>
       </c>
       <c r="G479" s="4">
         <v>0.046489</v>
@@ -15397,13 +15397,13 @@
         <v>971</v>
       </c>
       <c r="D483" s="4">
-        <v>241.98</v>
+        <v>240.15</v>
       </c>
       <c r="E483" s="5">
-        <v>0</v>
+        <v>-1.83</v>
       </c>
       <c r="F483" s="6">
-        <v>0</v>
+        <v>-0.0076</v>
       </c>
       <c r="G483" s="4">
         <v>0.410055</v>
@@ -15493,13 +15493,13 @@
         <v>979</v>
       </c>
       <c r="D487" s="4">
-        <v>545.96</v>
+        <v>545.5</v>
       </c>
       <c r="E487" s="5">
-        <v>0</v>
+        <v>-0.46</v>
       </c>
       <c r="F487" s="6">
-        <v>0</v>
+        <v>-0.0008</v>
       </c>
       <c r="G487" s="4">
         <v>1.329756</v>
@@ -15565,13 +15565,13 @@
         <v>985</v>
       </c>
       <c r="D490" s="4">
-        <v>103.22</v>
-      </c>
-      <c r="E490" s="5">
-        <v>0</v>
-      </c>
-      <c r="F490" s="6">
-        <v>0</v>
+        <v>103.7</v>
+      </c>
+      <c r="E490" s="12">
+        <v>0.48</v>
+      </c>
+      <c r="F490" s="13">
+        <v>0.0047</v>
       </c>
       <c r="G490" s="4">
         <v>0.110666</v>
@@ -15763,13 +15763,13 @@
         <v>1001</v>
       </c>
       <c r="D498" s="4">
-        <v>41.45</v>
+        <v>41.01</v>
       </c>
       <c r="E498" s="5">
-        <v>0</v>
+        <v>-0.44</v>
       </c>
       <c r="F498" s="6">
-        <v>0</v>
+        <v>-0.0106</v>
       </c>
       <c r="G498" s="4">
         <v>0.017322</v>
@@ -16053,13 +16053,13 @@
         <v>1025</v>
       </c>
       <c r="D510" s="4">
-        <v>48.73</v>
-      </c>
-      <c r="E510" s="5">
-        <v>0</v>
-      </c>
-      <c r="F510" s="6">
-        <v>0</v>
+        <v>48.88</v>
+      </c>
+      <c r="E510" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="F510" s="13">
+        <v>0.0031</v>
       </c>
       <c r="G510" s="4">
         <v>0.487775</v>
@@ -16125,13 +16125,13 @@
         <v>1031</v>
       </c>
       <c r="D513" s="7">
-        <v>47.18</v>
-      </c>
-      <c r="E513" s="8">
-        <v>0</v>
-      </c>
-      <c r="F513" s="9">
-        <v>0</v>
+        <v>47.22</v>
+      </c>
+      <c r="E513" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="F513" s="11">
+        <v>0.0008</v>
       </c>
       <c r="G513" s="7">
         <v>0.032209</v>
@@ -16221,13 +16221,13 @@
         <v>1039</v>
       </c>
       <c r="D517" s="7">
-        <v>172.08</v>
+        <v>172</v>
       </c>
       <c r="E517" s="8">
-        <v>0</v>
+        <v>-0.08</v>
       </c>
       <c r="F517" s="9">
-        <v>0</v>
+        <v>-0.0005</v>
       </c>
       <c r="G517" s="7">
         <v>0.026871</v>
@@ -16245,13 +16245,13 @@
         <v>1041</v>
       </c>
       <c r="D518" s="4">
-        <v>34.42</v>
+        <v>34.08</v>
       </c>
       <c r="E518" s="5">
-        <v>0</v>
+        <v>-0.34</v>
       </c>
       <c r="F518" s="6">
-        <v>0</v>
+        <v>-0.0099</v>
       </c>
       <c r="G518" s="4">
         <v>0.107098</v>
@@ -16367,13 +16367,13 @@
         <v>1051</v>
       </c>
       <c r="D523" s="4">
-        <v>86.67</v>
-      </c>
-      <c r="E523" s="5">
-        <v>0</v>
-      </c>
-      <c r="F523" s="6">
-        <v>0</v>
+        <v>87.43</v>
+      </c>
+      <c r="E523" s="12">
+        <v>0.76</v>
+      </c>
+      <c r="F523" s="13">
+        <v>0.0088</v>
       </c>
       <c r="G523" s="4">
         <v>0.040932</v>
@@ -16439,13 +16439,13 @@
         <v>1057</v>
       </c>
       <c r="D526" s="4">
-        <v>129.62</v>
+        <v>129.25</v>
       </c>
       <c r="E526" s="5">
-        <v>0</v>
+        <v>-0.37</v>
       </c>
       <c r="F526" s="6">
-        <v>0</v>
+        <v>-0.0029</v>
       </c>
       <c r="G526" s="4">
         <v>0.071053</v>

</xml_diff>

<commit_message>
Rel 10.00 Labour Day$
</commit_message>
<xml_diff>
--- a/Images/Stock Market Listing.xlsx
+++ b/Images/Stock Market Listing.xlsx
@@ -3835,7 +3835,7 @@
         <v>0.068806</v>
       </c>
       <c r="H7" s="4">
-        <v>0.201</v>
+        <v>0.202</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -4005,7 +4005,7 @@
         <v>0.164909</v>
       </c>
       <c r="H14" s="4">
-        <v>0.48</v>
+        <v>0.495</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -4031,7 +4031,7 @@
         <v>0.534434</v>
       </c>
       <c r="H15" s="4">
-        <v>1.557</v>
+        <v>1.572</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -4081,7 +4081,7 @@
         <v>0.404434</v>
       </c>
       <c r="H17" s="7">
-        <v>1.172</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -4177,7 +4177,7 @@
       </c>
       <c r="G21" s="7"/>
       <c r="H21" s="7">
-        <v>0.476</v>
+        <v>0.478</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -4299,7 +4299,7 @@
         <v>0.061547</v>
       </c>
       <c r="H26" s="4">
-        <v>0.193</v>
+        <v>0.192</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -4397,7 +4397,7 @@
         <v>1.966524</v>
       </c>
       <c r="H30" s="4">
-        <v>3.451</v>
+        <v>3.478</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -4423,7 +4423,7 @@
         <v>1.829744</v>
       </c>
       <c r="H31" s="4">
-        <v>3.649</v>
+        <v>3.678</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -4437,13 +4437,13 @@
         <v>69</v>
       </c>
       <c r="D32" s="7">
-        <v>55.57</v>
-      </c>
-      <c r="E32" s="8">
-        <v>0</v>
-      </c>
-      <c r="F32" s="9">
-        <v>0</v>
+        <v>55.65</v>
+      </c>
+      <c r="E32" s="10">
+        <v>0.08</v>
+      </c>
+      <c r="F32" s="11">
+        <v>0.0014</v>
       </c>
       <c r="G32" s="7">
         <v>0.277714</v>
@@ -4473,7 +4473,7 @@
         <v>3.491132</v>
       </c>
       <c r="H33" s="7">
-        <v>7.124</v>
+        <v>6.409</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -4571,7 +4571,7 @@
         <v>0.142375</v>
       </c>
       <c r="H37" s="7">
-        <v>0.415</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -4741,7 +4741,7 @@
         <v>0.36938</v>
       </c>
       <c r="H44" s="7">
-        <v>1.065</v>
+        <v>1.092</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -4791,7 +4791,7 @@
         <v>0.232629</v>
       </c>
       <c r="H46" s="4">
-        <v>0.674</v>
+        <v>0.679</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -4865,7 +4865,7 @@
         <v>6.997923</v>
       </c>
       <c r="H49" s="7">
-        <v>12.928</v>
+        <v>13.038</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -4891,7 +4891,7 @@
         <v>0.28092</v>
       </c>
       <c r="H50" s="4">
-        <v>0.813</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -5035,7 +5035,7 @@
       </c>
       <c r="G56" s="7"/>
       <c r="H56" s="7">
-        <v>0.308</v>
+        <v>0.318</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -5059,7 +5059,7 @@
       </c>
       <c r="G57" s="7"/>
       <c r="H57" s="7">
-        <v>0.295</v>
+        <v>0.267</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -5133,7 +5133,7 @@
         <v>0.11847</v>
       </c>
       <c r="H60" s="7">
-        <v>0.346</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -5159,7 +5159,7 @@
         <v>0.266218</v>
       </c>
       <c r="H61" s="7">
-        <v>0.775</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -5231,7 +5231,7 @@
       </c>
       <c r="G64" s="7"/>
       <c r="H64" s="7">
-        <v>0.234</v>
+        <v>0.252</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -5521,7 +5521,7 @@
         <v>0.085085</v>
       </c>
       <c r="H76" s="7">
-        <v>0.248</v>
+        <v>0.256</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -5595,7 +5595,7 @@
         <v>0.262699</v>
       </c>
       <c r="H79" s="4">
-        <v>0.761</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -5717,7 +5717,7 @@
         <v>0.659688</v>
       </c>
       <c r="H84" s="7">
-        <v>1.905</v>
+        <v>1.909</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -5959,7 +5959,7 @@
         <v>0.215088</v>
       </c>
       <c r="H94" s="4">
-        <v>0.62</v>
+        <v>0.633</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -6009,7 +6009,7 @@
         <v>0.120982</v>
       </c>
       <c r="H96" s="7">
-        <v>0.354</v>
+        <v>0.352</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -6467,7 +6467,7 @@
         <v>0.151814</v>
       </c>
       <c r="H115" s="4">
-        <v>0.64</v>
+        <v>0.622</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -6637,7 +6637,7 @@
         <v>0.099938</v>
       </c>
       <c r="H122" s="4">
-        <v>0.342</v>
+        <v>0.346</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -6663,7 +6663,7 @@
         <v>0.589326</v>
       </c>
       <c r="H123" s="4">
-        <v>1.689</v>
+        <v>1.711</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -6809,7 +6809,7 @@
         <v>0.121349</v>
       </c>
       <c r="H129" s="7">
-        <v>0.354</v>
+        <v>0.357</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -6859,7 +6859,7 @@
         <v>0.520617</v>
       </c>
       <c r="H131" s="4">
-        <v>1.515</v>
+        <v>1.512</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -6969,13 +6969,13 @@
         <v>277</v>
       </c>
       <c r="D136" s="7">
-        <v>246.09</v>
-      </c>
-      <c r="E136" s="8">
-        <v>0</v>
-      </c>
-      <c r="F136" s="9">
-        <v>0</v>
+        <v>246.3</v>
+      </c>
+      <c r="E136" s="10">
+        <v>0.21</v>
+      </c>
+      <c r="F136" s="11">
+        <v>0.0009</v>
       </c>
       <c r="G136" s="7">
         <v>0.113164</v>
@@ -7005,7 +7005,7 @@
         <v>0.054945</v>
       </c>
       <c r="H137" s="7">
-        <v>0.161</v>
+        <v>0.163</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
@@ -7055,7 +7055,7 @@
         <v>0.068595</v>
       </c>
       <c r="H139" s="4">
-        <v>0.222</v>
+        <v>0.227</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
@@ -7069,13 +7069,13 @@
         <v>285</v>
       </c>
       <c r="D140" s="7">
-        <v>35.19</v>
-      </c>
-      <c r="E140" s="8">
-        <v>0</v>
-      </c>
-      <c r="F140" s="9">
-        <v>0</v>
+        <v>35.8</v>
+      </c>
+      <c r="E140" s="10">
+        <v>0.61</v>
+      </c>
+      <c r="F140" s="11">
+        <v>0.0173</v>
       </c>
       <c r="G140" s="7">
         <v>0.075042</v>
@@ -7129,7 +7129,7 @@
         <v>0.687775</v>
       </c>
       <c r="H142" s="4">
-        <v>2.002</v>
+        <v>1.982</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
@@ -7143,13 +7143,13 @@
         <v>291</v>
       </c>
       <c r="D143" s="4">
-        <v>28.79</v>
-      </c>
-      <c r="E143" s="5">
-        <v>0</v>
-      </c>
-      <c r="F143" s="6">
-        <v>0</v>
+        <v>29.19</v>
+      </c>
+      <c r="E143" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="F143" s="13">
+        <v>0.0139</v>
       </c>
       <c r="G143" s="4">
         <v>0.065091</v>
@@ -7177,7 +7177,7 @@
       </c>
       <c r="G144" s="7"/>
       <c r="H144" s="7">
-        <v>0.346</v>
+        <v>0.348</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
@@ -7441,7 +7441,7 @@
       </c>
       <c r="G155" s="4"/>
       <c r="H155" s="4">
-        <v>0.273</v>
+        <v>0.268</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
@@ -7539,7 +7539,7 @@
         <v>0.1099</v>
       </c>
       <c r="H159" s="4">
-        <v>0.322</v>
+        <v>0.333</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
@@ -7635,7 +7635,7 @@
       </c>
       <c r="G163" s="4"/>
       <c r="H163" s="4">
-        <v>0.136</v>
+        <v>0.135</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
@@ -7685,7 +7685,7 @@
         <v>0.103515</v>
       </c>
       <c r="H165" s="7">
-        <v>0.302</v>
+        <v>0.307</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
@@ -7723,13 +7723,13 @@
         <v>339</v>
       </c>
       <c r="D167" s="4">
-        <v>338</v>
-      </c>
-      <c r="E167" s="5">
-        <v>0</v>
-      </c>
-      <c r="F167" s="6">
-        <v>0</v>
+        <v>339.11</v>
+      </c>
+      <c r="E167" s="12">
+        <v>1.11</v>
+      </c>
+      <c r="F167" s="13">
+        <v>0.0033</v>
       </c>
       <c r="G167" s="4">
         <v>0.035914</v>
@@ -7771,13 +7771,13 @@
         <v>343</v>
       </c>
       <c r="D169" s="7">
-        <v>66.5</v>
-      </c>
-      <c r="E169" s="8">
-        <v>0</v>
-      </c>
-      <c r="F169" s="9">
-        <v>0</v>
+        <v>66.93</v>
+      </c>
+      <c r="E169" s="10">
+        <v>0.43</v>
+      </c>
+      <c r="F169" s="11">
+        <v>0.0065</v>
       </c>
       <c r="G169" s="7">
         <v>0.138127</v>
@@ -7843,13 +7843,13 @@
         <v>349</v>
       </c>
       <c r="D172" s="7">
-        <v>54.75</v>
-      </c>
-      <c r="E172" s="8">
-        <v>0</v>
-      </c>
-      <c r="F172" s="9">
-        <v>0</v>
+        <v>55.08</v>
+      </c>
+      <c r="E172" s="10">
+        <v>0.33</v>
+      </c>
+      <c r="F172" s="11">
+        <v>0.006</v>
       </c>
       <c r="G172" s="7">
         <v>0.063011</v>
@@ -7867,13 +7867,13 @@
         <v>351</v>
       </c>
       <c r="D173" s="7">
-        <v>116.76</v>
-      </c>
-      <c r="E173" s="8">
-        <v>0</v>
-      </c>
-      <c r="F173" s="9">
-        <v>0</v>
+        <v>117.12</v>
+      </c>
+      <c r="E173" s="10">
+        <v>0.36</v>
+      </c>
+      <c r="F173" s="11">
+        <v>0.0031</v>
       </c>
       <c r="G173" s="7">
         <v>0.190166</v>
@@ -7891,13 +7891,13 @@
         <v>353</v>
       </c>
       <c r="D174" s="4">
-        <v>264.99</v>
-      </c>
-      <c r="E174" s="5">
-        <v>0</v>
-      </c>
-      <c r="F174" s="6">
-        <v>0</v>
+        <v>267.5</v>
+      </c>
+      <c r="E174" s="12">
+        <v>2.51</v>
+      </c>
+      <c r="F174" s="13">
+        <v>0.0095</v>
       </c>
       <c r="G174" s="4">
         <v>0.043923</v>
@@ -7915,13 +7915,13 @@
         <v>355</v>
       </c>
       <c r="D175" s="4">
-        <v>102.67</v>
-      </c>
-      <c r="E175" s="5">
-        <v>0</v>
-      </c>
-      <c r="F175" s="6">
-        <v>0</v>
+        <v>107.8</v>
+      </c>
+      <c r="E175" s="12">
+        <v>5.13</v>
+      </c>
+      <c r="F175" s="13">
+        <v>0.05</v>
       </c>
       <c r="G175" s="4">
         <v>0.038232</v>
@@ -7939,13 +7939,13 @@
         <v>357</v>
       </c>
       <c r="D176" s="7">
-        <v>145.02</v>
-      </c>
-      <c r="E176" s="8">
-        <v>0</v>
-      </c>
-      <c r="F176" s="9">
-        <v>0</v>
+        <v>145.87</v>
+      </c>
+      <c r="E176" s="10">
+        <v>0.85</v>
+      </c>
+      <c r="F176" s="11">
+        <v>0.0059</v>
       </c>
       <c r="G176" s="7">
         <v>0.16208</v>
@@ -8109,13 +8109,13 @@
         <v>371</v>
       </c>
       <c r="D183" s="4">
-        <v>90.18</v>
-      </c>
-      <c r="E183" s="5">
-        <v>0</v>
-      </c>
-      <c r="F183" s="6">
-        <v>0</v>
+        <v>90.83</v>
+      </c>
+      <c r="E183" s="12">
+        <v>0.65</v>
+      </c>
+      <c r="F183" s="13">
+        <v>0.0072</v>
       </c>
       <c r="G183" s="4">
         <v>0.151733</v>
@@ -8157,13 +8157,13 @@
         <v>375</v>
       </c>
       <c r="D185" s="7">
-        <v>118.85</v>
-      </c>
-      <c r="E185" s="8">
-        <v>0</v>
-      </c>
-      <c r="F185" s="9">
-        <v>0</v>
+        <v>122.32</v>
+      </c>
+      <c r="E185" s="10">
+        <v>3.47</v>
+      </c>
+      <c r="F185" s="11">
+        <v>0.0292</v>
       </c>
       <c r="G185" s="7">
         <v>0.067566</v>
@@ -8325,13 +8325,13 @@
         <v>389</v>
       </c>
       <c r="D192" s="7">
-        <v>274.71</v>
-      </c>
-      <c r="E192" s="8">
-        <v>0</v>
-      </c>
-      <c r="F192" s="9">
-        <v>0</v>
+        <v>277</v>
+      </c>
+      <c r="E192" s="10">
+        <v>2.29</v>
+      </c>
+      <c r="F192" s="11">
+        <v>0.0083</v>
       </c>
       <c r="G192" s="7">
         <v>0.030987</v>
@@ -8409,7 +8409,7 @@
         <v>0.129961</v>
       </c>
       <c r="H195" s="4">
-        <v>0.381</v>
+        <v>0.385</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.25">
@@ -8471,13 +8471,13 @@
         <v>401</v>
       </c>
       <c r="D198" s="4">
-        <v>190</v>
-      </c>
-      <c r="E198" s="5">
-        <v>0</v>
-      </c>
-      <c r="F198" s="6">
-        <v>0</v>
+        <v>191</v>
+      </c>
+      <c r="E198" s="12">
+        <v>1</v>
+      </c>
+      <c r="F198" s="13">
+        <v>0.0053</v>
       </c>
       <c r="G198" s="4">
         <v>0.076547</v>
@@ -8495,13 +8495,13 @@
         <v>403</v>
       </c>
       <c r="D199" s="4">
-        <v>85.25</v>
-      </c>
-      <c r="E199" s="5">
-        <v>0</v>
-      </c>
-      <c r="F199" s="6">
-        <v>0</v>
+        <v>85.5</v>
+      </c>
+      <c r="E199" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="F199" s="13">
+        <v>0.0029</v>
       </c>
       <c r="G199" s="4">
         <v>1.018833</v>
@@ -8627,7 +8627,7 @@
         <v>0.090766</v>
       </c>
       <c r="H204" s="7">
-        <v>0.266</v>
+        <v>0.268</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.25">
@@ -8665,13 +8665,13 @@
         <v>417</v>
       </c>
       <c r="D206" s="4">
-        <v>117.06</v>
-      </c>
-      <c r="E206" s="5">
-        <v>0</v>
-      </c>
-      <c r="F206" s="6">
-        <v>0</v>
+        <v>117.77</v>
+      </c>
+      <c r="E206" s="12">
+        <v>0.71</v>
+      </c>
+      <c r="F206" s="13">
+        <v>0.0061</v>
       </c>
       <c r="G206" s="4">
         <v>0.023405</v>
@@ -8689,13 +8689,13 @@
         <v>419</v>
       </c>
       <c r="D207" s="4">
-        <v>99.15</v>
-      </c>
-      <c r="E207" s="5">
-        <v>0</v>
-      </c>
-      <c r="F207" s="6">
-        <v>0</v>
+        <v>99.2</v>
+      </c>
+      <c r="E207" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="F207" s="13">
+        <v>0.0005</v>
       </c>
       <c r="G207" s="4">
         <v>0.174078</v>
@@ -8797,7 +8797,7 @@
         <v>0.171646</v>
       </c>
       <c r="H211" s="4">
-        <v>0.549</v>
+        <v>0.537</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.25">
@@ -8847,7 +8847,7 @@
         <v>0.115046</v>
       </c>
       <c r="H213" s="7">
-        <v>0.399</v>
+        <v>0.391</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.25">
@@ -8981,13 +8981,13 @@
         <v>443</v>
       </c>
       <c r="D219" s="4">
-        <v>40.55</v>
-      </c>
-      <c r="E219" s="5">
-        <v>0</v>
-      </c>
-      <c r="F219" s="6">
-        <v>0</v>
+        <v>40.56</v>
+      </c>
+      <c r="E219" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="F219" s="13">
+        <v>0.0002</v>
       </c>
       <c r="G219" s="4">
         <v>0.168931</v>
@@ -9005,13 +9005,13 @@
         <v>445</v>
       </c>
       <c r="D220" s="7">
-        <v>109.74</v>
-      </c>
-      <c r="E220" s="8">
-        <v>0</v>
-      </c>
-      <c r="F220" s="9">
-        <v>0</v>
+        <v>115</v>
+      </c>
+      <c r="E220" s="10">
+        <v>5.26</v>
+      </c>
+      <c r="F220" s="11">
+        <v>0.0479</v>
       </c>
       <c r="G220" s="7">
         <v>0.045793</v>
@@ -9053,13 +9053,13 @@
         <v>449</v>
       </c>
       <c r="D222" s="4">
-        <v>219.38</v>
-      </c>
-      <c r="E222" s="5">
-        <v>0</v>
-      </c>
-      <c r="F222" s="6">
-        <v>0</v>
+        <v>220.4</v>
+      </c>
+      <c r="E222" s="12">
+        <v>1.02</v>
+      </c>
+      <c r="F222" s="13">
+        <v>0.0046</v>
       </c>
       <c r="G222" s="4">
         <v>0.040486</v>
@@ -9209,7 +9209,7 @@
         <v>0.213112</v>
       </c>
       <c r="H228" s="7">
-        <v>0.62</v>
+        <v>0.626</v>
       </c>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.25">
@@ -9223,13 +9223,13 @@
         <v>463</v>
       </c>
       <c r="D229" s="7">
-        <v>136.98</v>
-      </c>
-      <c r="E229" s="8">
-        <v>0</v>
-      </c>
-      <c r="F229" s="9">
-        <v>0</v>
+        <v>137.55</v>
+      </c>
+      <c r="E229" s="10">
+        <v>0.57</v>
+      </c>
+      <c r="F229" s="11">
+        <v>0.0042</v>
       </c>
       <c r="G229" s="7">
         <v>0.113074</v>
@@ -9619,7 +9619,7 @@
         <v>0.359285</v>
       </c>
       <c r="H245" s="7">
-        <v>1.046</v>
+        <v>1.116</v>
       </c>
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.25">
@@ -9813,7 +9813,7 @@
         <v>0.104887</v>
       </c>
       <c r="H253" s="7">
-        <v>0.303</v>
+        <v>0.305</v>
       </c>
     </row>
     <row r="254" spans="1:8" x14ac:dyDescent="0.25">
@@ -9911,7 +9911,7 @@
         <v>0.130506</v>
       </c>
       <c r="H257" s="7">
-        <v>0.382</v>
+        <v>0.392</v>
       </c>
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.25">
@@ -9985,7 +9985,7 @@
         <v>0.526386</v>
       </c>
       <c r="H260" s="7">
-        <v>1.532</v>
+        <v>1.492</v>
       </c>
     </row>
     <row r="261" spans="1:8" x14ac:dyDescent="0.25">
@@ -9999,13 +9999,13 @@
         <v>527</v>
       </c>
       <c r="D261" s="7">
-        <v>115.81</v>
-      </c>
-      <c r="E261" s="8">
-        <v>0</v>
-      </c>
-      <c r="F261" s="9">
-        <v>0</v>
+        <v>116.66</v>
+      </c>
+      <c r="E261" s="10">
+        <v>0.85</v>
+      </c>
+      <c r="F261" s="11">
+        <v>0.0073</v>
       </c>
       <c r="G261" s="7">
         <v>0.184647</v>
@@ -10023,13 +10023,13 @@
         <v>529</v>
       </c>
       <c r="D262" s="4">
-        <v>132.21</v>
-      </c>
-      <c r="E262" s="5">
-        <v>0</v>
-      </c>
-      <c r="F262" s="6">
-        <v>0</v>
+        <v>132.6</v>
+      </c>
+      <c r="E262" s="12">
+        <v>0.39</v>
+      </c>
+      <c r="F262" s="13">
+        <v>0.0029</v>
       </c>
       <c r="G262" s="4">
         <v>0.33596</v>
@@ -10131,7 +10131,7 @@
         <v>0.347434</v>
       </c>
       <c r="H266" s="4">
-        <v>1.011</v>
+        <v>0.997</v>
       </c>
     </row>
     <row r="267" spans="1:8" x14ac:dyDescent="0.25">
@@ -10157,7 +10157,7 @@
         <v>0.240168</v>
       </c>
       <c r="H267" s="4">
-        <v>0.699</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="268" spans="1:8" x14ac:dyDescent="0.25">
@@ -10171,13 +10171,13 @@
         <v>541</v>
       </c>
       <c r="D268" s="7">
-        <v>18.38</v>
-      </c>
-      <c r="E268" s="8">
-        <v>0</v>
-      </c>
-      <c r="F268" s="9">
-        <v>0</v>
+        <v>18.62</v>
+      </c>
+      <c r="E268" s="10">
+        <v>0.24</v>
+      </c>
+      <c r="F268" s="11">
+        <v>0.0131</v>
       </c>
       <c r="G268" s="7">
         <v>0.018117</v>
@@ -10195,13 +10195,13 @@
         <v>543</v>
       </c>
       <c r="D269" s="7">
-        <v>53.73</v>
+        <v>52.91</v>
       </c>
       <c r="E269" s="8">
-        <v>0</v>
+        <v>-0.82</v>
       </c>
       <c r="F269" s="9">
-        <v>0</v>
+        <v>-0.0153</v>
       </c>
       <c r="G269" s="7">
         <v>0.044504</v>
@@ -10243,13 +10243,13 @@
         <v>547</v>
       </c>
       <c r="D271" s="4">
-        <v>136.93</v>
-      </c>
-      <c r="E271" s="5">
-        <v>0</v>
-      </c>
-      <c r="F271" s="6">
-        <v>0</v>
+        <v>137.91</v>
+      </c>
+      <c r="E271" s="12">
+        <v>0.98</v>
+      </c>
+      <c r="F271" s="13">
+        <v>0.0072</v>
       </c>
       <c r="G271" s="4">
         <v>0.042014</v>
@@ -10277,7 +10277,7 @@
       </c>
       <c r="G272" s="7"/>
       <c r="H272" s="7">
-        <v>0.277</v>
+        <v>0.309</v>
       </c>
     </row>
     <row r="273" spans="1:8" x14ac:dyDescent="0.25">
@@ -10291,13 +10291,13 @@
         <v>551</v>
       </c>
       <c r="D273" s="7">
-        <v>119.36</v>
-      </c>
-      <c r="E273" s="8">
-        <v>0</v>
-      </c>
-      <c r="F273" s="9">
-        <v>0</v>
+        <v>119.9</v>
+      </c>
+      <c r="E273" s="10">
+        <v>0.54</v>
+      </c>
+      <c r="F273" s="11">
+        <v>0.0045</v>
       </c>
       <c r="G273" s="7">
         <v>1.00596</v>
@@ -10363,13 +10363,13 @@
         <v>557</v>
       </c>
       <c r="D276" s="7">
-        <v>180.46</v>
-      </c>
-      <c r="E276" s="8">
-        <v>0</v>
-      </c>
-      <c r="F276" s="9">
-        <v>0</v>
+        <v>180.58</v>
+      </c>
+      <c r="E276" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="F276" s="11">
+        <v>0.0007</v>
       </c>
       <c r="G276" s="7">
         <v>1.332921</v>
@@ -10411,13 +10411,13 @@
         <v>561</v>
       </c>
       <c r="D278" s="4">
-        <v>31.52</v>
-      </c>
-      <c r="E278" s="5">
-        <v>0</v>
-      </c>
-      <c r="F278" s="6">
-        <v>0</v>
+        <v>31.55</v>
+      </c>
+      <c r="E278" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="F278" s="13">
+        <v>0.001</v>
       </c>
       <c r="G278" s="4">
         <v>0.029217</v>
@@ -10447,7 +10447,7 @@
         <v>0.13895</v>
       </c>
       <c r="H279" s="4">
-        <v>0.403</v>
+        <v>0.405</v>
       </c>
     </row>
     <row r="280" spans="1:8" x14ac:dyDescent="0.25">
@@ -10495,7 +10495,7 @@
       </c>
       <c r="G281" s="7"/>
       <c r="H281" s="7">
-        <v>0.433</v>
+        <v>0.446</v>
       </c>
     </row>
     <row r="282" spans="1:8" x14ac:dyDescent="0.25">
@@ -10641,7 +10641,7 @@
         <v>0.085049</v>
       </c>
       <c r="H287" s="4">
-        <v>0.429</v>
+        <v>0.439</v>
       </c>
     </row>
     <row r="288" spans="1:8" x14ac:dyDescent="0.25">
@@ -10679,13 +10679,13 @@
         <v>583</v>
       </c>
       <c r="D289" s="7">
-        <v>232.26</v>
+        <v>230</v>
       </c>
       <c r="E289" s="8">
-        <v>0</v>
+        <v>-2.26</v>
       </c>
       <c r="F289" s="9">
-        <v>0</v>
+        <v>-0.0097</v>
       </c>
       <c r="G289" s="7">
         <v>0.129218</v>
@@ -10763,7 +10763,7 @@
         <v>0.186522</v>
       </c>
       <c r="H292" s="7">
-        <v>0.543</v>
+        <v>0.546</v>
       </c>
     </row>
     <row r="293" spans="1:8" x14ac:dyDescent="0.25">
@@ -10849,13 +10849,13 @@
         <v>597</v>
       </c>
       <c r="D296" s="7">
-        <v>76.49</v>
-      </c>
-      <c r="E296" s="8">
-        <v>0</v>
-      </c>
-      <c r="F296" s="9">
-        <v>0</v>
+        <v>77.4</v>
+      </c>
+      <c r="E296" s="10">
+        <v>0.91</v>
+      </c>
+      <c r="F296" s="11">
+        <v>0.0119</v>
       </c>
       <c r="G296" s="7">
         <v>0.05669</v>
@@ -10873,13 +10873,13 @@
         <v>599</v>
       </c>
       <c r="D297" s="7">
-        <v>60.15</v>
-      </c>
-      <c r="E297" s="8">
-        <v>0</v>
-      </c>
-      <c r="F297" s="9">
-        <v>0</v>
+        <v>60.29</v>
+      </c>
+      <c r="E297" s="10">
+        <v>0.14</v>
+      </c>
+      <c r="F297" s="11">
+        <v>0.0023</v>
       </c>
       <c r="G297" s="7">
         <v>0.029343</v>
@@ -10897,13 +10897,13 @@
         <v>601</v>
       </c>
       <c r="D298" s="4">
-        <v>311.96</v>
-      </c>
-      <c r="E298" s="5">
-        <v>0</v>
-      </c>
-      <c r="F298" s="6">
-        <v>0</v>
+        <v>314.93</v>
+      </c>
+      <c r="E298" s="12">
+        <v>2.97</v>
+      </c>
+      <c r="F298" s="13">
+        <v>0.0095</v>
       </c>
       <c r="G298" s="4">
         <v>0.445854</v>
@@ -11051,7 +11051,7 @@
       </c>
       <c r="G304" s="7"/>
       <c r="H304" s="7">
-        <v>0.359</v>
+        <v>0.368</v>
       </c>
     </row>
     <row r="305" spans="1:8" x14ac:dyDescent="0.25">
@@ -11065,13 +11065,13 @@
         <v>615</v>
       </c>
       <c r="D305" s="7">
-        <v>10.06</v>
-      </c>
-      <c r="E305" s="8">
-        <v>0</v>
-      </c>
-      <c r="F305" s="9">
-        <v>0</v>
+        <v>10.1</v>
+      </c>
+      <c r="E305" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="F305" s="11">
+        <v>0.004</v>
       </c>
       <c r="G305" s="7">
         <v>0.026718</v>
@@ -11137,13 +11137,13 @@
         <v>621</v>
       </c>
       <c r="D308" s="7">
-        <v>41.04</v>
-      </c>
-      <c r="E308" s="8">
-        <v>0</v>
-      </c>
-      <c r="F308" s="9">
-        <v>0</v>
+        <v>41.1</v>
+      </c>
+      <c r="E308" s="10">
+        <v>0.06</v>
+      </c>
+      <c r="F308" s="11">
+        <v>0.0015</v>
       </c>
       <c r="G308" s="7">
         <v>0.043774</v>
@@ -11161,13 +11161,13 @@
         <v>623</v>
       </c>
       <c r="D309" s="7">
-        <v>421.25</v>
-      </c>
-      <c r="E309" s="8">
-        <v>0</v>
-      </c>
-      <c r="F309" s="9">
-        <v>0</v>
+        <v>421.54</v>
+      </c>
+      <c r="E309" s="10">
+        <v>0.29</v>
+      </c>
+      <c r="F309" s="11">
+        <v>0.0007</v>
       </c>
       <c r="G309" s="7">
         <v>0.097176</v>
@@ -11185,13 +11185,13 @@
         <v>625</v>
       </c>
       <c r="D310" s="4">
-        <v>24.92</v>
-      </c>
-      <c r="E310" s="5">
-        <v>0</v>
-      </c>
-      <c r="F310" s="6">
-        <v>0</v>
+        <v>25.02</v>
+      </c>
+      <c r="E310" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="F310" s="13">
+        <v>0.004</v>
       </c>
       <c r="G310" s="4">
         <v>0.055202</v>
@@ -11209,13 +11209,13 @@
         <v>627</v>
       </c>
       <c r="D311" s="4">
-        <v>87.26</v>
-      </c>
-      <c r="E311" s="5">
-        <v>0</v>
-      </c>
-      <c r="F311" s="6">
-        <v>0</v>
+        <v>87.27</v>
+      </c>
+      <c r="E311" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="F311" s="13">
+        <v>0.0001</v>
       </c>
       <c r="G311" s="4">
         <v>0.14332</v>
@@ -11269,7 +11269,7 @@
         <v>0.13883</v>
       </c>
       <c r="H313" s="7">
-        <v>0.484</v>
+        <v>0.487</v>
       </c>
     </row>
     <row r="314" spans="1:8" x14ac:dyDescent="0.25">
@@ -11341,7 +11341,7 @@
       </c>
       <c r="G316" s="7"/>
       <c r="H316" s="7">
-        <v>0.414</v>
+        <v>0.412</v>
       </c>
     </row>
     <row r="317" spans="1:8" x14ac:dyDescent="0.25">
@@ -11415,7 +11415,7 @@
         <v>0.063623</v>
       </c>
       <c r="H319" s="4">
-        <v>0.187</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="320" spans="1:8" x14ac:dyDescent="0.25">
@@ -11501,13 +11501,13 @@
         <v>651</v>
       </c>
       <c r="D323" s="4">
-        <v>104.36</v>
-      </c>
-      <c r="E323" s="5">
-        <v>0</v>
-      </c>
-      <c r="F323" s="6">
-        <v>0</v>
+        <v>105.16</v>
+      </c>
+      <c r="E323" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="F323" s="13">
+        <v>0.0077</v>
       </c>
       <c r="G323" s="4">
         <v>0.397193</v>
@@ -11535,7 +11535,7 @@
       </c>
       <c r="G324" s="7"/>
       <c r="H324" s="7">
-        <v>0.421</v>
+        <v>0.413</v>
       </c>
     </row>
     <row r="325" spans="1:8" x14ac:dyDescent="0.25">
@@ -11549,13 +11549,13 @@
         <v>655</v>
       </c>
       <c r="D325" s="7">
-        <v>88.69</v>
-      </c>
-      <c r="E325" s="8">
-        <v>0</v>
-      </c>
-      <c r="F325" s="9">
-        <v>0</v>
+        <v>88.95</v>
+      </c>
+      <c r="E325" s="10">
+        <v>0.26</v>
+      </c>
+      <c r="F325" s="11">
+        <v>0.0029</v>
       </c>
       <c r="G325" s="7">
         <v>0.617504</v>
@@ -11573,13 +11573,13 @@
         <v>657</v>
       </c>
       <c r="D326" s="4">
-        <v>65.68</v>
-      </c>
-      <c r="E326" s="5">
-        <v>0</v>
-      </c>
-      <c r="F326" s="6">
-        <v>0</v>
+        <v>66.21</v>
+      </c>
+      <c r="E326" s="12">
+        <v>0.53</v>
+      </c>
+      <c r="F326" s="13">
+        <v>0.0081</v>
       </c>
       <c r="G326" s="4">
         <v>0.131238</v>
@@ -11609,7 +11609,7 @@
         <v>1.311042</v>
       </c>
       <c r="H327" s="4">
-        <v>3.444</v>
+        <v>3.513</v>
       </c>
     </row>
     <row r="328" spans="1:8" x14ac:dyDescent="0.25">
@@ -11659,7 +11659,7 @@
         <v>0.10421</v>
       </c>
       <c r="H329" s="7">
-        <v>0.304</v>
+        <v>0.305</v>
       </c>
     </row>
     <row r="330" spans="1:8" x14ac:dyDescent="0.25">
@@ -11685,7 +11685,7 @@
         <v>0.216192</v>
       </c>
       <c r="H330" s="4">
-        <v>0.631</v>
+        <v>0.642</v>
       </c>
     </row>
     <row r="331" spans="1:8" x14ac:dyDescent="0.25">
@@ -11711,7 +11711,7 @@
         <v>5.990018</v>
       </c>
       <c r="H331" s="4">
-        <v>10.512</v>
+        <v>10.543</v>
       </c>
     </row>
     <row r="332" spans="1:8" x14ac:dyDescent="0.25">
@@ -11761,7 +11761,7 @@
         <v>0.138479</v>
       </c>
       <c r="H333" s="7">
-        <v>0.461</v>
+        <v>0.455</v>
       </c>
     </row>
     <row r="334" spans="1:8" x14ac:dyDescent="0.25">
@@ -11775,13 +11775,13 @@
         <v>673</v>
       </c>
       <c r="D334" s="4">
-        <v>141.06</v>
+        <v>141</v>
       </c>
       <c r="E334" s="5">
-        <v>0</v>
+        <v>-0.06</v>
       </c>
       <c r="F334" s="6">
-        <v>0</v>
+        <v>-0.0004</v>
       </c>
       <c r="G334" s="4">
         <v>0.020131</v>
@@ -11859,7 +11859,7 @@
         <v>0.253593</v>
       </c>
       <c r="H337" s="7">
-        <v>0.738</v>
+        <v>0.753</v>
       </c>
     </row>
     <row r="338" spans="1:8" x14ac:dyDescent="0.25">
@@ -11909,7 +11909,7 @@
         <v>0.091044</v>
       </c>
       <c r="H339" s="4">
-        <v>0.373</v>
+        <v>0.381</v>
       </c>
     </row>
     <row r="340" spans="1:8" x14ac:dyDescent="0.25">
@@ -11947,13 +11947,13 @@
         <v>687</v>
       </c>
       <c r="D341" s="7">
-        <v>80.59</v>
-      </c>
-      <c r="E341" s="8">
-        <v>0</v>
-      </c>
-      <c r="F341" s="9">
-        <v>0</v>
+        <v>80.85</v>
+      </c>
+      <c r="E341" s="10">
+        <v>0.26</v>
+      </c>
+      <c r="F341" s="11">
+        <v>0.0032</v>
       </c>
       <c r="G341" s="7">
         <v>0.326285</v>
@@ -12079,7 +12079,7 @@
         <v>1.364146</v>
       </c>
       <c r="H346" s="4">
-        <v>3.369</v>
+        <v>3.307</v>
       </c>
     </row>
     <row r="347" spans="1:8" x14ac:dyDescent="0.25">
@@ -12129,7 +12129,7 @@
         <v>0.130087</v>
       </c>
       <c r="H348" s="7">
-        <v>0.374</v>
+        <v>0.377</v>
       </c>
     </row>
     <row r="349" spans="1:8" x14ac:dyDescent="0.25">
@@ -12201,7 +12201,7 @@
       </c>
       <c r="G351" s="4"/>
       <c r="H351" s="4">
-        <v>0.154</v>
+        <v>0.168</v>
       </c>
     </row>
     <row r="352" spans="1:8" x14ac:dyDescent="0.25">
@@ -12265,13 +12265,13 @@
         <v>713</v>
       </c>
       <c r="D354" s="4">
-        <v>72.85</v>
+        <v>72.8</v>
       </c>
       <c r="E354" s="5">
-        <v>0</v>
+        <v>-0.05</v>
       </c>
       <c r="F354" s="6">
-        <v>0</v>
+        <v>-0.0007</v>
       </c>
       <c r="G354" s="4">
         <v>0.161025</v>
@@ -12529,13 +12529,13 @@
         <v>735</v>
       </c>
       <c r="D365" s="7">
-        <v>20.03</v>
-      </c>
-      <c r="E365" s="8">
-        <v>0</v>
-      </c>
-      <c r="F365" s="9">
-        <v>0</v>
+        <v>20.08</v>
+      </c>
+      <c r="E365" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="F365" s="11">
+        <v>0.0025</v>
       </c>
       <c r="G365" s="7">
         <v>0.023724</v>
@@ -12553,13 +12553,13 @@
         <v>737</v>
       </c>
       <c r="D366" s="4">
-        <v>154.78</v>
-      </c>
-      <c r="E366" s="5">
-        <v>0</v>
-      </c>
-      <c r="F366" s="6">
-        <v>0</v>
+        <v>154.9</v>
+      </c>
+      <c r="E366" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="F366" s="13">
+        <v>0.0007</v>
       </c>
       <c r="G366" s="4">
         <v>0.120596</v>
@@ -12589,7 +12589,7 @@
         <v>0.115632</v>
       </c>
       <c r="H367" s="4">
-        <v>0.333</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="368" spans="1:8" x14ac:dyDescent="0.25">
@@ -12603,13 +12603,13 @@
         <v>741</v>
       </c>
       <c r="D368" s="7">
-        <v>63.33</v>
-      </c>
-      <c r="E368" s="8">
-        <v>0</v>
-      </c>
-      <c r="F368" s="9">
-        <v>0</v>
+        <v>63.83</v>
+      </c>
+      <c r="E368" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F368" s="11">
+        <v>0.0079</v>
       </c>
       <c r="G368" s="7">
         <v>0.082006</v>
@@ -12661,7 +12661,7 @@
       </c>
       <c r="G370" s="4"/>
       <c r="H370" s="4">
-        <v>0.157</v>
+        <v>0.149</v>
       </c>
     </row>
     <row r="371" spans="1:8" x14ac:dyDescent="0.25">
@@ -12687,7 +12687,7 @@
         <v>0.075365</v>
       </c>
       <c r="H371" s="4">
-        <v>0.27</v>
+        <v>0.271</v>
       </c>
     </row>
     <row r="372" spans="1:8" x14ac:dyDescent="0.25">
@@ -12701,13 +12701,13 @@
         <v>749</v>
       </c>
       <c r="D372" s="7">
-        <v>76.13</v>
-      </c>
-      <c r="E372" s="8">
-        <v>0</v>
-      </c>
-      <c r="F372" s="9">
-        <v>0</v>
+        <v>77</v>
+      </c>
+      <c r="E372" s="10">
+        <v>0.87</v>
+      </c>
+      <c r="F372" s="11">
+        <v>0.0114</v>
       </c>
       <c r="G372" s="7">
         <v>0.045372</v>
@@ -12809,7 +12809,7 @@
         <v>0.081197</v>
       </c>
       <c r="H376" s="7">
-        <v>0.237</v>
+        <v>0.243</v>
       </c>
     </row>
     <row r="377" spans="1:8" x14ac:dyDescent="0.25">
@@ -12847,13 +12847,13 @@
         <v>761</v>
       </c>
       <c r="D378" s="4">
-        <v>127.99</v>
-      </c>
-      <c r="E378" s="5">
-        <v>0</v>
-      </c>
-      <c r="F378" s="6">
-        <v>0</v>
+        <v>128.03</v>
+      </c>
+      <c r="E378" s="12">
+        <v>0.04</v>
+      </c>
+      <c r="F378" s="13">
+        <v>0.0003</v>
       </c>
       <c r="G378" s="4">
         <v>0.085381</v>
@@ -12871,13 +12871,13 @@
         <v>763</v>
       </c>
       <c r="D379" s="4">
-        <v>28.31</v>
+        <v>28.3</v>
       </c>
       <c r="E379" s="5">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="F379" s="6">
-        <v>0</v>
+        <v>-0.0004</v>
       </c>
       <c r="G379" s="4">
         <v>0.060888</v>
@@ -12977,7 +12977,7 @@
       </c>
       <c r="G383" s="4"/>
       <c r="H383" s="4">
-        <v>0.466</v>
+        <v>0.465</v>
       </c>
     </row>
     <row r="384" spans="1:8" x14ac:dyDescent="0.25">
@@ -13051,7 +13051,7 @@
         <v>0.29609</v>
       </c>
       <c r="H386" s="4">
-        <v>0.862</v>
+        <v>0.861</v>
       </c>
     </row>
     <row r="387" spans="1:8" x14ac:dyDescent="0.25">
@@ -13175,7 +13175,7 @@
         <v>0.677702</v>
       </c>
       <c r="H391" s="4">
-        <v>1.972</v>
+        <v>1.997</v>
       </c>
     </row>
     <row r="392" spans="1:8" x14ac:dyDescent="0.25">
@@ -13213,13 +13213,13 @@
         <v>791</v>
       </c>
       <c r="D393" s="7">
-        <v>49.07</v>
+        <v>48.65</v>
       </c>
       <c r="E393" s="8">
-        <v>0</v>
+        <v>-0.42</v>
       </c>
       <c r="F393" s="9">
-        <v>0</v>
+        <v>-0.0086</v>
       </c>
       <c r="G393" s="7">
         <v>0.782426</v>
@@ -13237,13 +13237,13 @@
         <v>793</v>
       </c>
       <c r="D394" s="4">
-        <v>100</v>
-      </c>
-      <c r="E394" s="5">
-        <v>0</v>
-      </c>
-      <c r="F394" s="6">
-        <v>0</v>
+        <v>100.72</v>
+      </c>
+      <c r="E394" s="12">
+        <v>0.72</v>
+      </c>
+      <c r="F394" s="13">
+        <v>0.0072</v>
       </c>
       <c r="G394" s="4">
         <v>0.438427</v>
@@ -13261,13 +13261,13 @@
         <v>795</v>
       </c>
       <c r="D395" s="4">
-        <v>86.76</v>
-      </c>
-      <c r="E395" s="5">
-        <v>0</v>
-      </c>
-      <c r="F395" s="6">
-        <v>0</v>
+        <v>86.85</v>
+      </c>
+      <c r="E395" s="12">
+        <v>0.09</v>
+      </c>
+      <c r="F395" s="13">
+        <v>0.001</v>
       </c>
       <c r="G395" s="4">
         <v>0.112337</v>
@@ -13295,7 +13295,7 @@
       </c>
       <c r="G396" s="7"/>
       <c r="H396" s="7">
-        <v>0.135</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="397" spans="1:8" x14ac:dyDescent="0.25">
@@ -13333,13 +13333,13 @@
         <v>801</v>
       </c>
       <c r="D398" s="4">
-        <v>232.47</v>
-      </c>
-      <c r="E398" s="5">
-        <v>0</v>
-      </c>
-      <c r="F398" s="6">
-        <v>0</v>
+        <v>234</v>
+      </c>
+      <c r="E398" s="12">
+        <v>1.53</v>
+      </c>
+      <c r="F398" s="13">
+        <v>0.0066</v>
       </c>
       <c r="G398" s="4">
         <v>0.146551</v>
@@ -13453,13 +13453,13 @@
         <v>811</v>
       </c>
       <c r="D403" s="4">
-        <v>160.29</v>
-      </c>
-      <c r="E403" s="5">
-        <v>0</v>
-      </c>
-      <c r="F403" s="6">
-        <v>0</v>
+        <v>160.9</v>
+      </c>
+      <c r="E403" s="12">
+        <v>0.61</v>
+      </c>
+      <c r="F403" s="13">
+        <v>0.0038</v>
       </c>
       <c r="G403" s="4">
         <v>0.353334</v>
@@ -13477,13 +13477,13 @@
         <v>813</v>
       </c>
       <c r="D404" s="7">
-        <v>108.51</v>
-      </c>
-      <c r="E404" s="8">
-        <v>0</v>
-      </c>
-      <c r="F404" s="9">
-        <v>0</v>
+        <v>110</v>
+      </c>
+      <c r="E404" s="10">
+        <v>1.49</v>
+      </c>
+      <c r="F404" s="11">
+        <v>0.0137</v>
       </c>
       <c r="G404" s="7">
         <v>0.116727</v>
@@ -13525,13 +13525,13 @@
         <v>817</v>
       </c>
       <c r="D406" s="4">
-        <v>371.5</v>
-      </c>
-      <c r="E406" s="5">
-        <v>0</v>
-      </c>
-      <c r="F406" s="6">
-        <v>0</v>
+        <v>372.72</v>
+      </c>
+      <c r="E406" s="12">
+        <v>1.22</v>
+      </c>
+      <c r="F406" s="13">
+        <v>0.0033</v>
       </c>
       <c r="G406" s="4">
         <v>0.167146</v>
@@ -13609,7 +13609,7 @@
         <v>0.460914</v>
       </c>
       <c r="H409" s="7">
-        <v>1.341</v>
+        <v>1.324</v>
       </c>
     </row>
     <row r="410" spans="1:8" x14ac:dyDescent="0.25">
@@ -13623,13 +13623,13 @@
         <v>825</v>
       </c>
       <c r="D410" s="4">
-        <v>115.98</v>
-      </c>
-      <c r="E410" s="5">
-        <v>0</v>
-      </c>
-      <c r="F410" s="6">
-        <v>0</v>
+        <v>116.9</v>
+      </c>
+      <c r="E410" s="12">
+        <v>0.92</v>
+      </c>
+      <c r="F410" s="13">
+        <v>0.0079</v>
       </c>
       <c r="G410" s="4">
         <v>0.046736</v>
@@ -13803,7 +13803,7 @@
         <v>0.198973</v>
       </c>
       <c r="H417" s="7">
-        <v>0.579</v>
+        <v>0.591</v>
       </c>
     </row>
     <row r="418" spans="1:8" x14ac:dyDescent="0.25">
@@ -13817,13 +13817,13 @@
         <v>841</v>
       </c>
       <c r="D418" s="4">
-        <v>20.72</v>
-      </c>
-      <c r="E418" s="5">
-        <v>0</v>
-      </c>
-      <c r="F418" s="6">
-        <v>0</v>
+        <v>20.89</v>
+      </c>
+      <c r="E418" s="12">
+        <v>0.17</v>
+      </c>
+      <c r="F418" s="13">
+        <v>0.0082</v>
       </c>
       <c r="G418" s="4">
         <v>0.056015</v>
@@ -13841,13 +13841,13 @@
         <v>843</v>
       </c>
       <c r="D419" s="4">
-        <v>134.27</v>
+        <v>134.22</v>
       </c>
       <c r="E419" s="5">
-        <v>0</v>
+        <v>-0.05</v>
       </c>
       <c r="F419" s="6">
-        <v>0</v>
+        <v>-0.0004</v>
       </c>
       <c r="G419" s="4">
         <v>0.079803</v>
@@ -14035,13 +14035,13 @@
         <v>859</v>
       </c>
       <c r="D427" s="4">
-        <v>376.5</v>
-      </c>
-      <c r="E427" s="5">
-        <v>0</v>
-      </c>
-      <c r="F427" s="6">
-        <v>0</v>
+        <v>376.61</v>
+      </c>
+      <c r="E427" s="12">
+        <v>0.11</v>
+      </c>
+      <c r="F427" s="13">
+        <v>0.0003</v>
       </c>
       <c r="G427" s="4">
         <v>0.377332</v>
@@ -14155,13 +14155,13 @@
         <v>869</v>
       </c>
       <c r="D432" s="7">
-        <v>39.01</v>
-      </c>
-      <c r="E432" s="8">
-        <v>0</v>
-      </c>
-      <c r="F432" s="9">
-        <v>0</v>
+        <v>39.02</v>
+      </c>
+      <c r="E432" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="F432" s="11">
+        <v>0.0003</v>
       </c>
       <c r="G432" s="7">
         <v>0.155347</v>
@@ -14213,7 +14213,7 @@
       </c>
       <c r="G434" s="4"/>
       <c r="H434" s="4">
-        <v>0.192</v>
+        <v>0.202</v>
       </c>
     </row>
     <row r="435" spans="1:8" x14ac:dyDescent="0.25">
@@ -14251,13 +14251,13 @@
         <v>877</v>
       </c>
       <c r="D436" s="7">
-        <v>161.36</v>
-      </c>
-      <c r="E436" s="8">
-        <v>0</v>
-      </c>
-      <c r="F436" s="9">
-        <v>0</v>
+        <v>161.39</v>
+      </c>
+      <c r="E436" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="F436" s="11">
+        <v>0.0002</v>
       </c>
       <c r="G436" s="7">
         <v>0.145859</v>
@@ -14299,13 +14299,13 @@
         <v>881</v>
       </c>
       <c r="D438" s="4">
-        <v>274.96</v>
-      </c>
-      <c r="E438" s="5">
-        <v>0</v>
-      </c>
-      <c r="F438" s="6">
-        <v>0</v>
+        <v>275.1</v>
+      </c>
+      <c r="E438" s="12">
+        <v>0.14</v>
+      </c>
+      <c r="F438" s="13">
+        <v>0.0005</v>
       </c>
       <c r="G438" s="4">
         <v>0.186684</v>
@@ -14347,13 +14347,13 @@
         <v>885</v>
       </c>
       <c r="D440" s="7">
-        <v>118</v>
-      </c>
-      <c r="E440" s="8">
-        <v>0</v>
-      </c>
-      <c r="F440" s="9">
-        <v>0</v>
+        <v>118.78</v>
+      </c>
+      <c r="E440" s="10">
+        <v>0.78</v>
+      </c>
+      <c r="F440" s="11">
+        <v>0.0066</v>
       </c>
       <c r="G440" s="7">
         <v>0.112412</v>
@@ -14381,7 +14381,7 @@
       </c>
       <c r="G441" s="7"/>
       <c r="H441" s="7">
-        <v>0.2</v>
+        <v>0.199</v>
       </c>
     </row>
     <row r="442" spans="1:8" x14ac:dyDescent="0.25">
@@ -14407,7 +14407,7 @@
         <v>0.053425</v>
       </c>
       <c r="H442" s="4">
-        <v>0.155</v>
+        <v>0.156</v>
       </c>
     </row>
     <row r="443" spans="1:8" x14ac:dyDescent="0.25">
@@ -14469,13 +14469,13 @@
         <v>895</v>
       </c>
       <c r="D445" s="7">
-        <v>73.39</v>
-      </c>
-      <c r="E445" s="8">
-        <v>0</v>
-      </c>
-      <c r="F445" s="9">
-        <v>0</v>
+        <v>73.75</v>
+      </c>
+      <c r="E445" s="10">
+        <v>0.36</v>
+      </c>
+      <c r="F445" s="11">
+        <v>0.0049</v>
       </c>
       <c r="G445" s="7">
         <v>0.221064</v>
@@ -14527,7 +14527,7 @@
       </c>
       <c r="G447" s="4"/>
       <c r="H447" s="4">
-        <v>0.161</v>
+        <v>0.163</v>
       </c>
     </row>
     <row r="448" spans="1:8" x14ac:dyDescent="0.25">
@@ -14541,13 +14541,13 @@
         <v>901</v>
       </c>
       <c r="D448" s="7">
-        <v>120.15</v>
-      </c>
-      <c r="E448" s="8">
-        <v>0</v>
-      </c>
-      <c r="F448" s="9">
-        <v>0</v>
+        <v>122.1</v>
+      </c>
+      <c r="E448" s="10">
+        <v>1.95</v>
+      </c>
+      <c r="F448" s="11">
+        <v>0.0162</v>
       </c>
       <c r="G448" s="7">
         <v>0.056655</v>
@@ -14577,7 +14577,7 @@
         <v>0.243111</v>
       </c>
       <c r="H449" s="7">
-        <v>0.708</v>
+        <v>0.722</v>
       </c>
     </row>
     <row r="450" spans="1:8" x14ac:dyDescent="0.25">
@@ -14591,13 +14591,13 @@
         <v>905</v>
       </c>
       <c r="D450" s="4">
-        <v>66.97</v>
-      </c>
-      <c r="E450" s="5">
-        <v>0</v>
-      </c>
-      <c r="F450" s="6">
-        <v>0</v>
+        <v>67.5</v>
+      </c>
+      <c r="E450" s="12">
+        <v>0.53</v>
+      </c>
+      <c r="F450" s="13">
+        <v>0.0079</v>
       </c>
       <c r="G450" s="4">
         <v>0.069206</v>
@@ -14675,7 +14675,7 @@
         <v>0.127836</v>
       </c>
       <c r="H453" s="7">
-        <v>0.371</v>
+        <v>0.369</v>
       </c>
     </row>
     <row r="454" spans="1:8" x14ac:dyDescent="0.25">
@@ -14725,7 +14725,7 @@
         <v>0.214359</v>
       </c>
       <c r="H455" s="4">
-        <v>1.327</v>
+        <v>1.293</v>
       </c>
     </row>
     <row r="456" spans="1:8" x14ac:dyDescent="0.25">
@@ -14835,13 +14835,13 @@
         <v>925</v>
       </c>
       <c r="D460" s="7">
-        <v>32.92</v>
+        <v>32.8</v>
       </c>
       <c r="E460" s="8">
-        <v>0</v>
+        <v>-0.12</v>
       </c>
       <c r="F460" s="9">
-        <v>0</v>
+        <v>-0.0036</v>
       </c>
       <c r="G460" s="7">
         <v>0.024336</v>
@@ -14859,13 +14859,13 @@
         <v>927</v>
       </c>
       <c r="D461" s="7">
-        <v>228.65</v>
-      </c>
-      <c r="E461" s="8">
-        <v>0</v>
-      </c>
-      <c r="F461" s="9">
-        <v>0</v>
+        <v>229</v>
+      </c>
+      <c r="E461" s="10">
+        <v>0.35</v>
+      </c>
+      <c r="F461" s="11">
+        <v>0.0015</v>
       </c>
       <c r="G461" s="7">
         <v>0.312576</v>
@@ -14883,13 +14883,13 @@
         <v>929</v>
       </c>
       <c r="D462" s="4">
-        <v>431.55</v>
+        <v>431</v>
       </c>
       <c r="E462" s="5">
-        <v>0</v>
+        <v>-0.55</v>
       </c>
       <c r="F462" s="6">
-        <v>0</v>
+        <v>-0.0013</v>
       </c>
       <c r="G462" s="4">
         <v>0.058217</v>
@@ -14967,7 +14967,7 @@
         <v>2.02629</v>
       </c>
       <c r="H465" s="7">
-        <v>4.39</v>
+        <v>4.56</v>
       </c>
     </row>
     <row r="466" spans="1:8" x14ac:dyDescent="0.25">
@@ -14993,7 +14993,7 @@
         <v>0.448208</v>
       </c>
       <c r="H466" s="4">
-        <v>1.304</v>
+        <v>1.322</v>
       </c>
     </row>
     <row r="467" spans="1:8" x14ac:dyDescent="0.25">
@@ -15079,13 +15079,13 @@
         <v>945</v>
       </c>
       <c r="D470" s="4">
-        <v>139.89</v>
-      </c>
-      <c r="E470" s="5">
-        <v>0</v>
-      </c>
-      <c r="F470" s="6">
-        <v>0</v>
+        <v>139.92</v>
+      </c>
+      <c r="E470" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="F470" s="13">
+        <v>0.0002</v>
       </c>
       <c r="G470" s="4">
         <v>0.093866</v>
@@ -15127,13 +15127,13 @@
         <v>949</v>
       </c>
       <c r="D472" s="7">
-        <v>171.06</v>
-      </c>
-      <c r="E472" s="8">
-        <v>0</v>
-      </c>
-      <c r="F472" s="9">
-        <v>0</v>
+        <v>171.14</v>
+      </c>
+      <c r="E472" s="10">
+        <v>0.08</v>
+      </c>
+      <c r="F472" s="11">
+        <v>0.0005</v>
       </c>
       <c r="G472" s="7">
         <v>0.116161</v>
@@ -15175,13 +15175,13 @@
         <v>953</v>
       </c>
       <c r="D474" s="4">
-        <v>48.35</v>
-      </c>
-      <c r="E474" s="5">
-        <v>0</v>
-      </c>
-      <c r="F474" s="6">
-        <v>0</v>
+        <v>48.75</v>
+      </c>
+      <c r="E474" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="F474" s="13">
+        <v>0.0083</v>
       </c>
       <c r="G474" s="4">
         <v>0.184424</v>
@@ -15271,13 +15271,13 @@
         <v>961</v>
       </c>
       <c r="D478" s="4">
-        <v>48.56</v>
-      </c>
-      <c r="E478" s="5">
-        <v>0</v>
-      </c>
-      <c r="F478" s="6">
-        <v>0</v>
+        <v>49.3</v>
+      </c>
+      <c r="E478" s="12">
+        <v>0.74</v>
+      </c>
+      <c r="F478" s="13">
+        <v>0.0152</v>
       </c>
       <c r="G478" s="4">
         <v>0.186499</v>
@@ -15367,13 +15367,13 @@
         <v>969</v>
       </c>
       <c r="D482" s="4">
-        <v>14.19</v>
-      </c>
-      <c r="E482" s="5">
-        <v>0</v>
-      </c>
-      <c r="F482" s="6">
-        <v>0</v>
+        <v>14.43</v>
+      </c>
+      <c r="E482" s="12">
+        <v>0.24</v>
+      </c>
+      <c r="F482" s="13">
+        <v>0.0169</v>
       </c>
       <c r="G482" s="4">
         <v>0.007825</v>
@@ -15463,13 +15463,13 @@
         <v>977</v>
       </c>
       <c r="D486" s="4">
-        <v>316.52</v>
-      </c>
-      <c r="E486" s="5">
-        <v>0</v>
-      </c>
-      <c r="F486" s="6">
-        <v>0</v>
+        <v>318.15</v>
+      </c>
+      <c r="E486" s="12">
+        <v>1.63</v>
+      </c>
+      <c r="F486" s="13">
+        <v>0.0051</v>
       </c>
       <c r="G486" s="4">
         <v>0.063325</v>
@@ -15487,13 +15487,13 @@
         <v>979</v>
       </c>
       <c r="D487" s="4">
-        <v>508.55</v>
-      </c>
-      <c r="E487" s="5">
-        <v>0</v>
-      </c>
-      <c r="F487" s="6">
-        <v>0</v>
+        <v>509.2</v>
+      </c>
+      <c r="E487" s="12">
+        <v>0.65</v>
+      </c>
+      <c r="F487" s="13">
+        <v>0.0013</v>
       </c>
       <c r="G487" s="4">
         <v>1.363147</v>
@@ -15559,13 +15559,13 @@
         <v>985</v>
       </c>
       <c r="D490" s="4">
-        <v>111.48</v>
-      </c>
-      <c r="E490" s="5">
-        <v>0</v>
-      </c>
-      <c r="F490" s="6">
-        <v>0</v>
+        <v>111.75</v>
+      </c>
+      <c r="E490" s="12">
+        <v>0.27</v>
+      </c>
+      <c r="F490" s="13">
+        <v>0.0024</v>
       </c>
       <c r="G490" s="4">
         <v>0.129865</v>
@@ -15619,7 +15619,7 @@
         <v>0.055766</v>
       </c>
       <c r="H492" s="7">
-        <v>0.184</v>
+        <v>0.166</v>
       </c>
     </row>
     <row r="493" spans="1:8" x14ac:dyDescent="0.25">
@@ -15645,7 +15645,7 @@
         <v>0.094331</v>
       </c>
       <c r="H493" s="7">
-        <v>0.276</v>
+        <v>0.277</v>
       </c>
     </row>
     <row r="494" spans="1:8" x14ac:dyDescent="0.25">
@@ -15695,7 +15695,7 @@
         <v>0.188095</v>
       </c>
       <c r="H495" s="4">
-        <v>0.549</v>
+        <v>0.585</v>
       </c>
     </row>
     <row r="496" spans="1:8" x14ac:dyDescent="0.25">
@@ -15853,13 +15853,13 @@
         <v>1009</v>
       </c>
       <c r="D502" s="4">
-        <v>100.05</v>
-      </c>
-      <c r="E502" s="5">
-        <v>0</v>
-      </c>
-      <c r="F502" s="6">
-        <v>0</v>
+        <v>101.5</v>
+      </c>
+      <c r="E502" s="12">
+        <v>1.45</v>
+      </c>
+      <c r="F502" s="13">
+        <v>0.0145</v>
       </c>
       <c r="G502" s="4">
         <v>0.089128</v>
@@ -15889,7 +15889,7 @@
         <v>0.087891</v>
       </c>
       <c r="H503" s="4">
-        <v>0.309</v>
+        <v>0.308</v>
       </c>
     </row>
     <row r="504" spans="1:8" x14ac:dyDescent="0.25">
@@ -15903,13 +15903,13 @@
         <v>1013</v>
       </c>
       <c r="D504" s="7">
-        <v>152.99</v>
-      </c>
-      <c r="E504" s="8">
-        <v>0</v>
-      </c>
-      <c r="F504" s="9">
-        <v>0</v>
+        <v>153.06</v>
+      </c>
+      <c r="E504" s="10">
+        <v>0.07</v>
+      </c>
+      <c r="F504" s="11">
+        <v>0.0005</v>
       </c>
       <c r="G504" s="7">
         <v>0.609888</v>
@@ -15975,13 +15975,13 @@
         <v>1019</v>
       </c>
       <c r="D507" s="4">
-        <v>164.44</v>
+        <v>164.02</v>
       </c>
       <c r="E507" s="5">
-        <v>0</v>
+        <v>-0.42</v>
       </c>
       <c r="F507" s="6">
-        <v>0</v>
+        <v>-0.0026</v>
       </c>
       <c r="G507" s="4">
         <v>0.179797</v>
@@ -16023,13 +16023,13 @@
         <v>1023</v>
       </c>
       <c r="D509" s="7">
-        <v>43.63</v>
-      </c>
-      <c r="E509" s="8">
-        <v>0</v>
-      </c>
-      <c r="F509" s="9">
-        <v>0</v>
+        <v>43.85</v>
+      </c>
+      <c r="E509" s="10">
+        <v>0.22</v>
+      </c>
+      <c r="F509" s="11">
+        <v>0.005</v>
       </c>
       <c r="G509" s="7">
         <v>0.484407</v>
@@ -16047,13 +16047,13 @@
         <v>1025</v>
       </c>
       <c r="D510" s="4">
-        <v>90.81</v>
+        <v>90.51</v>
       </c>
       <c r="E510" s="5">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
       <c r="F510" s="6">
-        <v>0</v>
+        <v>-0.0033</v>
       </c>
       <c r="G510" s="4">
         <v>0.113245</v>
@@ -16071,13 +16071,13 @@
         <v>1027</v>
       </c>
       <c r="D511" s="4">
-        <v>315.06</v>
+        <v>313</v>
       </c>
       <c r="E511" s="5">
-        <v>0</v>
+        <v>-2.06</v>
       </c>
       <c r="F511" s="6">
-        <v>0</v>
+        <v>-0.0065</v>
       </c>
       <c r="G511" s="4">
         <v>0.066133</v>
@@ -16095,13 +16095,13 @@
         <v>1029</v>
       </c>
       <c r="D512" s="7">
-        <v>49.53</v>
+        <v>48.3</v>
       </c>
       <c r="E512" s="8">
-        <v>0</v>
+        <v>-1.23</v>
       </c>
       <c r="F512" s="9">
-        <v>0</v>
+        <v>-0.0248</v>
       </c>
       <c r="G512" s="7">
         <v>0.036496</v>
@@ -16167,13 +16167,13 @@
         <v>1035</v>
       </c>
       <c r="D515" s="4">
-        <v>41.22</v>
-      </c>
-      <c r="E515" s="5">
-        <v>0</v>
-      </c>
-      <c r="F515" s="6">
-        <v>0</v>
+        <v>41.63</v>
+      </c>
+      <c r="E515" s="12">
+        <v>0.41</v>
+      </c>
+      <c r="F515" s="13">
+        <v>0.0099</v>
       </c>
       <c r="G515" s="4">
         <v>0.086368</v>
@@ -16191,13 +16191,13 @@
         <v>1037</v>
       </c>
       <c r="D516" s="7">
-        <v>181.52</v>
-      </c>
-      <c r="E516" s="8">
-        <v>0</v>
-      </c>
-      <c r="F516" s="9">
-        <v>0</v>
+        <v>185.71</v>
+      </c>
+      <c r="E516" s="10">
+        <v>4.19</v>
+      </c>
+      <c r="F516" s="11">
+        <v>0.0231</v>
       </c>
       <c r="G516" s="7">
         <v>0.030993</v>
@@ -16215,13 +16215,13 @@
         <v>1039</v>
       </c>
       <c r="D517" s="7">
-        <v>34.29</v>
+        <v>34.01</v>
       </c>
       <c r="E517" s="8">
-        <v>0</v>
+        <v>-0.28</v>
       </c>
       <c r="F517" s="9">
-        <v>0</v>
+        <v>-0.0082</v>
       </c>
       <c r="G517" s="7">
         <v>0.116348</v>
@@ -16273,7 +16273,7 @@
       </c>
       <c r="G519" s="4"/>
       <c r="H519" s="4">
-        <v>0.339</v>
+        <v>0.341</v>
       </c>
     </row>
     <row r="520" spans="1:8" x14ac:dyDescent="0.25">
@@ -16323,7 +16323,7 @@
         <v>0.11085</v>
       </c>
       <c r="H521" s="7">
-        <v>0.327</v>
+        <v>0.335</v>
       </c>
     </row>
     <row r="522" spans="1:8" x14ac:dyDescent="0.25">
@@ -16457,13 +16457,13 @@
         <v>1059</v>
       </c>
       <c r="D527" s="4">
-        <v>177.25</v>
-      </c>
-      <c r="E527" s="5">
-        <v>0</v>
-      </c>
-      <c r="F527" s="6">
-        <v>0</v>
+        <v>178.5</v>
+      </c>
+      <c r="E527" s="12">
+        <v>1.25</v>
+      </c>
+      <c r="F527" s="13">
+        <v>0.0071</v>
       </c>
       <c r="G527" s="4">
         <v>0.236287</v>
@@ -16491,7 +16491,7 @@
       </c>
       <c r="G528" s="7"/>
       <c r="H528" s="7">
-        <v>0.2</v>
+        <v>0.203</v>
       </c>
     </row>
     <row r="529" spans="1:8" x14ac:dyDescent="0.25">
@@ -16515,7 +16515,7 @@
       </c>
       <c r="G529" s="7"/>
       <c r="H529" s="7">
-        <v>0.24</v>
+        <v>0.239</v>
       </c>
     </row>
     <row r="530" spans="1:8" x14ac:dyDescent="0.25">
@@ -16541,7 +16541,7 @@
         <v>0.09267</v>
       </c>
       <c r="H530" s="4">
-        <v>0.254</v>
+        <v>0.256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>